<commit_message>
added probs in table
</commit_message>
<xml_diff>
--- a/tables_plots/table_fine_mapping.xlsx
+++ b/tables_plots/table_fine_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,26 @@
           <t>chr</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_mean</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_std</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_median</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_samples</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -504,6 +524,18 @@
           <t>chr10</t>
         </is>
       </c>
+      <c r="H2" t="n">
+        <v>0.01603793496567938</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.05794792982282904</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.000309870533418</v>
+      </c>
+      <c r="K2" t="n">
+        <v>668</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -539,6 +571,18 @@
           <t>chr9</t>
         </is>
       </c>
+      <c r="H3" t="n">
+        <v>0.2650826103238722</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.05520277919403747</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.2720060174950369</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1065</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -574,6 +618,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H4" t="n">
+        <v>-0.02061823533022416</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01964678905325687</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.0254181746606881</v>
+      </c>
+      <c r="K4" t="n">
+        <v>36978</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -609,6 +665,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H5" t="n">
+        <v>-0.04474911429178613</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.01495691423501778</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-0.0484824113276277</v>
+      </c>
+      <c r="K5" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -644,6 +712,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H6" t="n">
+        <v>0.06317405297773764</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.05684670391539608</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.0506722973675428</v>
+      </c>
+      <c r="K6" t="n">
+        <v>285</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -679,6 +759,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H7" t="n">
+        <v>-0.02211802325627087</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.02136433981141503</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-0.0257277744520354</v>
+      </c>
+      <c r="K7" t="n">
+        <v>27136</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -714,6 +806,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H8" t="n">
+        <v>-0.1886719870376972</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.1076564051628712</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-0.2313363699753964</v>
+      </c>
+      <c r="K8" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -749,6 +853,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H9" t="n">
+        <v>-0.1325088443208639</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.00239733006487308</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-0.1332971773429439</v>
+      </c>
+      <c r="K9" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -784,6 +900,18 @@
           <t>chr8</t>
         </is>
       </c>
+      <c r="H10" t="n">
+        <v>0.02657588963425587</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1200299734152091</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.00677489475416395</v>
+      </c>
+      <c r="K10" t="n">
+        <v>902</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -819,6 +947,18 @@
           <t>chr8</t>
         </is>
       </c>
+      <c r="H11" t="n">
+        <v>0.008054595488127293</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.05792300338835416</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3.527061131661646e-05</v>
+      </c>
+      <c r="K11" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -854,6 +994,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H12" t="n">
+        <v>-0.0116035395789694</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.02555237604918957</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.0157108310070773</v>
+      </c>
+      <c r="K12" t="n">
+        <v>392123</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -889,6 +1041,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H13" t="n">
+        <v>0.02112058000943368</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.04195812000926728</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0176744092042852</v>
+      </c>
+      <c r="K13" t="n">
+        <v>755</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -924,6 +1088,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H14" t="n">
+        <v>0.07240635403043384</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.09174849479652503</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.00260770984377</v>
+      </c>
+      <c r="K14" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -959,6 +1135,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H15" t="n">
+        <v>-0.01164293497351661</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.02517480386191833</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-0.01573311724271995</v>
+      </c>
+      <c r="K15" t="n">
+        <v>394378</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -994,6 +1182,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H16" t="n">
+        <v>0.05555090371296323</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.07826594259621866</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0005814157596602</v>
+      </c>
+      <c r="K16" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1029,6 +1229,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H17" t="n">
+        <v>-0.01370129387070619</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.02333677221547618</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-0.0193954863883875</v>
+      </c>
+      <c r="K17" t="n">
+        <v>34786</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1064,6 +1276,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H18" t="n">
+        <v>0.08061360773006593</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.06772259390299649</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0735445606956977</v>
+      </c>
+      <c r="K18" t="n">
+        <v>271</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1099,6 +1323,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H19" t="n">
+        <v>0.002848141718346069</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.02558179432450362</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-0.0012338074059341</v>
+      </c>
+      <c r="K19" t="n">
+        <v>25287</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1134,6 +1370,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H20" t="n">
+        <v>-0.1593371915749837</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2086777729744027</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.2464226786367025</v>
+      </c>
+      <c r="K20" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1169,6 +1417,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H21" t="n">
+        <v>-0.1454155620917435</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.01945581826731453</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-0.1539731871090594</v>
+      </c>
+      <c r="K21" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1204,6 +1464,18 @@
           <t>chr17</t>
         </is>
       </c>
+      <c r="H22" t="n">
+        <v>0.003785101912323079</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.05990633516750271</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.004835053114270901</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1546</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1239,6 +1511,18 @@
           <t>chr17</t>
         </is>
       </c>
+      <c r="H23" t="n">
+        <v>-0.03679154899055308</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.07154148175801353</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-0.02762697476021845</v>
+      </c>
+      <c r="K23" t="n">
+        <v>8776</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1274,6 +1558,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H24" t="n">
+        <v>0.08737157075405125</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.06810444311479932</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.07585703022469706</v>
+      </c>
+      <c r="K24" t="n">
+        <v>322</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1309,6 +1605,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H25" t="n">
+        <v>-0.02151903132644405</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.02189495770855255</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-0.025199452815315</v>
+      </c>
+      <c r="K25" t="n">
+        <v>30769</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1344,6 +1652,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H26" t="n">
+        <v>0.8012563980959789</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.8012563980959789</v>
+      </c>
+      <c r="K26" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1379,6 +1699,18 @@
           <t>chr6</t>
         </is>
       </c>
+      <c r="H27" t="n">
+        <v>-0.1422853250329177</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.006702176462369657</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-0.1445393989897263</v>
+      </c>
+      <c r="K27" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1413,6 +1745,18 @@
         <is>
           <t>chr14</t>
         </is>
+      </c>
+      <c r="H28" t="n">
+        <v>0.02464890816420632</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.06949486463827942</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.00458961670881205</v>
+      </c>
+      <c r="K28" t="n">
+        <v>420084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fine mapping table
</commit_message>
<xml_diff>
--- a/tables_plots/table_fine_mapping.xlsx
+++ b/tables_plots/table_fine_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,50 +441,65 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ancestry tested</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ancestry of the population</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Start Position of the reduced significant region</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>End Position of the reduced significant region</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Number of significant SNPs</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ancestry tested</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ancestry of the population</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>OR (CI = 95%)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>p value</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>chr</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_mean</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_std</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_median</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_samples</t>
         </is>
@@ -498,42 +513,51 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>114596655</v>
+      </c>
+      <c r="E2" t="n">
+        <v>116330728</v>
+      </c>
+      <c r="F2" t="n">
+        <v>103</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>rs72826020</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>0.89809 (0.840833, 0.959245)</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="I2" t="n">
         <v>0.00138436</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>chr10</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="K2" t="n">
         <v>0.01603793496567938</v>
       </c>
-      <c r="I2" t="n">
+      <c r="L2" t="n">
         <v>0.05794792982282904</v>
       </c>
-      <c r="J2" t="n">
+      <c r="M2" t="n">
         <v>-0.000309870533418</v>
       </c>
-      <c r="K2" t="n">
+      <c r="N2" t="n">
         <v>668</v>
       </c>
     </row>
@@ -545,42 +569,51 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AFR</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>84405371</v>
+      </c>
+      <c r="E3" t="n">
+        <v>88296425</v>
+      </c>
+      <c r="F3" t="n">
+        <v>14</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>rs41307444</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>AFR</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>2.551 (1.40816, 4.62135)</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
         <v>0.00200839</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>chr9</t>
         </is>
       </c>
-      <c r="H3" t="n">
+      <c r="K3" t="n">
         <v>0.2650826103238722</v>
       </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
         <v>0.05520277919403747</v>
       </c>
-      <c r="J3" t="n">
+      <c r="M3" t="n">
         <v>0.2720060174950369</v>
       </c>
-      <c r="K3" t="n">
+      <c r="N3" t="n">
         <v>1065</v>
       </c>
     </row>
@@ -592,42 +625,51 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>30718180</v>
+      </c>
+      <c r="E4" t="n">
+        <v>31729925</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1693</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>rs6931921</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>0.844061 (0.80753, 0.882245)</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
         <v>5.917389999999999e-14</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>-0.02061823533022416</v>
       </c>
-      <c r="I4" t="n">
+      <c r="L4" t="n">
         <v>0.01964678905325687</v>
       </c>
-      <c r="J4" t="n">
+      <c r="M4" t="n">
         <v>-0.0254181746606881</v>
       </c>
-      <c r="K4" t="n">
+      <c r="N4" t="n">
         <v>36978</v>
       </c>
     </row>
@@ -639,42 +681,51 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>30809864</v>
+      </c>
+      <c r="E5" t="n">
+        <v>31141523</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>rs887468</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>0.0506881 (0.00296067, 0.867803)</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
         <v>0.0396085</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="K5" t="n">
         <v>-0.04474911429178613</v>
       </c>
-      <c r="I5" t="n">
+      <c r="L5" t="n">
         <v>0.01495691423501778</v>
       </c>
-      <c r="J5" t="n">
+      <c r="M5" t="n">
         <v>-0.0484824113276277</v>
       </c>
-      <c r="K5" t="n">
+      <c r="N5" t="n">
         <v>81</v>
       </c>
     </row>
@@ -686,42 +737,51 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>EAS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>32565979</v>
+      </c>
+      <c r="E6" t="n">
+        <v>32565979</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>rs28383172</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>EAS</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>1.53878 (1.03235, 2.29367)</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
         <v>0.0343209</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="K6" t="n">
         <v>0.06317405297773764</v>
       </c>
-      <c r="I6" t="n">
+      <c r="L6" t="n">
         <v>0.05684670391539608</v>
       </c>
-      <c r="J6" t="n">
+      <c r="M6" t="n">
         <v>0.0506722973675428</v>
       </c>
-      <c r="K6" t="n">
+      <c r="N6" t="n">
         <v>285</v>
       </c>
     </row>
@@ -733,42 +793,51 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>31435991</v>
+      </c>
+      <c r="E7" t="n">
+        <v>32565973</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1055</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>rs4248166</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>0.900401 (0.883096, 0.918046)</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
         <v>3.12314e-26</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="K7" t="n">
         <v>-0.02211802325627087</v>
       </c>
-      <c r="I7" t="n">
+      <c r="L7" t="n">
         <v>0.02136433981141503</v>
       </c>
-      <c r="J7" t="n">
+      <c r="M7" t="n">
         <v>-0.0257277744520354</v>
       </c>
-      <c r="K7" t="n">
+      <c r="N7" t="n">
         <v>27136</v>
       </c>
     </row>
@@ -780,42 +849,51 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>31578772</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31593476</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>rs2844477</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>0.216515 (0.0645403, 0.726346)</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
         <v>0.013223</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="K8" t="n">
         <v>-0.1886719870376972</v>
       </c>
-      <c r="I8" t="n">
+      <c r="L8" t="n">
         <v>0.1076564051628712</v>
       </c>
-      <c r="J8" t="n">
+      <c r="M8" t="n">
         <v>-0.2313363699753964</v>
       </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
         <v>22</v>
       </c>
     </row>
@@ -827,42 +905,51 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>31435991</v>
+      </c>
+      <c r="E9" t="n">
+        <v>32413557</v>
+      </c>
+      <c r="F9" t="n">
+        <v>77</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>rs7758128</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>0.0187251 (0.000562785, 0.623023)</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
         <v>0.0261095</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="K9" t="n">
         <v>-0.1325088443208639</v>
       </c>
-      <c r="I9" t="n">
+      <c r="L9" t="n">
         <v>0.00239733006487308</v>
       </c>
-      <c r="J9" t="n">
+      <c r="M9" t="n">
         <v>-0.1332971773429439</v>
       </c>
-      <c r="K9" t="n">
+      <c r="N9" t="n">
         <v>10</v>
       </c>
     </row>
@@ -874,42 +961,51 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>123760560</v>
+      </c>
+      <c r="E10" t="n">
+        <v>125664204</v>
+      </c>
+      <c r="F10" t="n">
+        <v>35</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>rs4128469</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>0.905172 (0.838937, 0.976637)</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
         <v>0.0101781</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
       </c>
-      <c r="H10" t="n">
+      <c r="K10" t="n">
         <v>0.02657588963425587</v>
       </c>
-      <c r="I10" t="n">
+      <c r="L10" t="n">
         <v>0.1200299734152091</v>
       </c>
-      <c r="J10" t="n">
+      <c r="M10" t="n">
         <v>0.00677489475416395</v>
       </c>
-      <c r="K10" t="n">
+      <c r="N10" t="n">
         <v>902</v>
       </c>
     </row>
@@ -921,42 +1017,51 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>124091971</v>
+      </c>
+      <c r="E11" t="n">
+        <v>124091971</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>rs4870843</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>129.955 (4.00638, 4215.35)</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
         <v>0.00611053</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="K11" t="n">
         <v>0.008054595488127293</v>
       </c>
-      <c r="I11" t="n">
+      <c r="L11" t="n">
         <v>0.05792300338835416</v>
       </c>
-      <c r="J11" t="n">
+      <c r="M11" t="n">
         <v>3.527061131661646e-05</v>
       </c>
-      <c r="K11" t="n">
+      <c r="N11" t="n">
         <v>70</v>
       </c>
     </row>
@@ -968,42 +1073,51 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>31207822</v>
+      </c>
+      <c r="E12" t="n">
+        <v>31678691</v>
+      </c>
+      <c r="F12" t="n">
+        <v>618</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>rs2248372</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>0.94514 (0.929624, 0.960916)</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
         <v>2.38222e-11</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H12" t="n">
+      <c r="K12" t="n">
         <v>-0.0116035395789694</v>
       </c>
-      <c r="I12" t="n">
+      <c r="L12" t="n">
         <v>0.02555237604918957</v>
       </c>
-      <c r="J12" t="n">
+      <c r="M12" t="n">
         <v>-0.0157108310070773</v>
       </c>
-      <c r="K12" t="n">
+      <c r="N12" t="n">
         <v>392123</v>
       </c>
     </row>
@@ -1015,42 +1129,51 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>31480923</v>
+      </c>
+      <c r="E13" t="n">
+        <v>31480923</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>rs3131633</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>1.42596 (1.2161, 1.67202)</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
         <v>1.24933e-05</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H13" t="n">
+      <c r="K13" t="n">
         <v>0.02112058000943368</v>
       </c>
-      <c r="I13" t="n">
+      <c r="L13" t="n">
         <v>0.04195812000926728</v>
       </c>
-      <c r="J13" t="n">
+      <c r="M13" t="n">
         <v>0.0176744092042852</v>
       </c>
-      <c r="K13" t="n">
+      <c r="N13" t="n">
         <v>755</v>
       </c>
     </row>
@@ -1062,42 +1185,51 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>31330546</v>
+      </c>
+      <c r="E14" t="n">
+        <v>31371430</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>rs2596548</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>23.4192 (1.7359, 315.951)</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
         <v>0.01753</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H14" t="n">
+      <c r="K14" t="n">
         <v>0.07240635403043384</v>
       </c>
-      <c r="I14" t="n">
+      <c r="L14" t="n">
         <v>0.09174849479652503</v>
       </c>
-      <c r="J14" t="n">
+      <c r="M14" t="n">
         <v>0.00260770984377</v>
       </c>
-      <c r="K14" t="n">
+      <c r="N14" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1109,42 +1241,51 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>31207822</v>
+      </c>
+      <c r="E15" t="n">
+        <v>31570670</v>
+      </c>
+      <c r="F15" t="n">
+        <v>531</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>rs2248372</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>0.944111 (0.928517, 0.959967)</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
         <v>1.3074e-11</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H15" t="n">
+      <c r="K15" t="n">
         <v>-0.01164293497351661</v>
       </c>
-      <c r="I15" t="n">
+      <c r="L15" t="n">
         <v>0.02517480386191833</v>
       </c>
-      <c r="J15" t="n">
+      <c r="M15" t="n">
         <v>-0.01573311724271995</v>
       </c>
-      <c r="K15" t="n">
+      <c r="N15" t="n">
         <v>394378</v>
       </c>
     </row>
@@ -1156,42 +1297,51 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>31218268</v>
+      </c>
+      <c r="E16" t="n">
+        <v>31570670</v>
+      </c>
+      <c r="F16" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>rs2596548</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>19.9215 (1.56414, 253.728)</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
         <v>0.0211924</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H16" t="n">
+      <c r="K16" t="n">
         <v>0.05555090371296323</v>
       </c>
-      <c r="I16" t="n">
+      <c r="L16" t="n">
         <v>0.07826594259621866</v>
       </c>
-      <c r="J16" t="n">
+      <c r="M16" t="n">
         <v>0.0005814157596602</v>
       </c>
-      <c r="K16" t="n">
+      <c r="N16" t="n">
         <v>33</v>
       </c>
     </row>
@@ -1203,42 +1353,51 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>30628082</v>
+      </c>
+      <c r="E17" t="n">
+        <v>31729925</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1790</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Affx-28441669</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>0.883837 (0.863265, 0.904898)</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
         <v>8.95268e-25</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H17" t="n">
+      <c r="K17" t="n">
         <v>-0.01370129387070619</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
         <v>0.02333677221547618</v>
       </c>
-      <c r="J17" t="n">
+      <c r="M17" t="n">
         <v>-0.0193954863883875</v>
       </c>
-      <c r="K17" t="n">
+      <c r="N17" t="n">
         <v>34786</v>
       </c>
     </row>
@@ -1250,42 +1409,51 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>EAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>31240771</v>
+      </c>
+      <c r="E18" t="n">
+        <v>31316699</v>
+      </c>
+      <c r="F18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>rs10484554</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>EAS</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>1.62357 (1.11497, 2.36417)</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
         <v>0.0114863</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H18" t="n">
+      <c r="K18" t="n">
         <v>0.08061360773006593</v>
       </c>
-      <c r="I18" t="n">
+      <c r="L18" t="n">
         <v>0.06772259390299649</v>
       </c>
-      <c r="J18" t="n">
+      <c r="M18" t="n">
         <v>0.0735445606956977</v>
       </c>
-      <c r="K18" t="n">
+      <c r="N18" t="n">
         <v>271</v>
       </c>
     </row>
@@ -1297,42 +1465,51 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>31229579</v>
+      </c>
+      <c r="E19" t="n">
+        <v>32565973</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1435</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>rs9266490</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>1.05014 (1.03172, 1.06888)</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
         <v>6.01662e-08</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H19" t="n">
+      <c r="K19" t="n">
         <v>0.002848141718346069</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
         <v>0.02558179432450362</v>
       </c>
-      <c r="J19" t="n">
+      <c r="M19" t="n">
         <v>-0.0012338074059341</v>
       </c>
-      <c r="K19" t="n">
+      <c r="N19" t="n">
         <v>25287</v>
       </c>
     </row>
@@ -1344,42 +1521,51 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>31266767</v>
+      </c>
+      <c r="E20" t="n">
+        <v>31628733</v>
+      </c>
+      <c r="F20" t="n">
+        <v>9</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>rs4394275</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>0.0346081 (0.00196079, 0.610838)</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
         <v>0.0216473</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H20" t="n">
+      <c r="K20" t="n">
         <v>-0.1593371915749837</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
         <v>0.2086777729744027</v>
       </c>
-      <c r="J20" t="n">
+      <c r="M20" t="n">
         <v>-0.2464226786367025</v>
       </c>
-      <c r="K20" t="n">
+      <c r="N20" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1391,42 +1577,51 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>31236800</v>
+      </c>
+      <c r="E21" t="n">
+        <v>32413557</v>
+      </c>
+      <c r="F21" t="n">
+        <v>86</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>rs13198903</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>0.0477015 (0.00332903, 0.683512)</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
         <v>0.0250848</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H21" t="n">
+      <c r="K21" t="n">
         <v>-0.1454155620917435</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
         <v>0.01945581826731453</v>
       </c>
-      <c r="J21" t="n">
+      <c r="M21" t="n">
         <v>-0.1539731871090594</v>
       </c>
-      <c r="K21" t="n">
+      <c r="N21" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1438,42 +1633,51 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1605567</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2307902</v>
+      </c>
+      <c r="F22" t="n">
+        <v>23</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>rs903160</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>0.987432 (0.976643, 0.99834)</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="I22" t="n">
         <v>0.0240458</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
       </c>
-      <c r="H22" t="n">
+      <c r="K22" t="n">
         <v>0.003785101912323079</v>
       </c>
-      <c r="I22" t="n">
+      <c r="L22" t="n">
         <v>0.05990633516750271</v>
       </c>
-      <c r="J22" t="n">
+      <c r="M22" t="n">
         <v>-0.004835053114270901</v>
       </c>
-      <c r="K22" t="n">
+      <c r="N22" t="n">
         <v>1546</v>
       </c>
     </row>
@@ -1485,42 +1689,51 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1795180</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2282779</v>
+      </c>
+      <c r="F23" t="n">
+        <v>17</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>rs62067003</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>0.894641 (0.819604, 0.976549)</t>
         </is>
       </c>
-      <c r="F23" t="n">
+      <c r="I23" t="n">
         <v>0.012742</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
       </c>
-      <c r="H23" t="n">
+      <c r="K23" t="n">
         <v>-0.03679154899055308</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
         <v>0.07154148175801353</v>
       </c>
-      <c r="J23" t="n">
+      <c r="M23" t="n">
         <v>-0.02762697476021845</v>
       </c>
-      <c r="K23" t="n">
+      <c r="N23" t="n">
         <v>8776</v>
       </c>
     </row>
@@ -1532,42 +1745,51 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>EAS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>32565979</v>
+      </c>
+      <c r="E24" t="n">
+        <v>32565979</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>rs28383172</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>EAS</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>1.71722 (1.1625, 2.53662)</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
         <v>0.00659873</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H24" t="n">
+      <c r="K24" t="n">
         <v>0.08737157075405125</v>
       </c>
-      <c r="I24" t="n">
+      <c r="L24" t="n">
         <v>0.06810444311479932</v>
       </c>
-      <c r="J24" t="n">
+      <c r="M24" t="n">
         <v>0.07585703022469706</v>
       </c>
-      <c r="K24" t="n">
+      <c r="N24" t="n">
         <v>322</v>
       </c>
     </row>
@@ -1579,42 +1801,51 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>32177880</v>
+      </c>
+      <c r="E25" t="n">
+        <v>32565973</v>
+      </c>
+      <c r="F25" t="n">
+        <v>528</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>rs4248166</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>0.903429 (0.886177, 0.921016)</t>
         </is>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
         <v>5.49011e-25</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H25" t="n">
+      <c r="K25" t="n">
         <v>-0.02151903132644405</v>
       </c>
-      <c r="I25" t="n">
+      <c r="L25" t="n">
         <v>0.02189495770855255</v>
       </c>
-      <c r="J25" t="n">
+      <c r="M25" t="n">
         <v>-0.025199452815315</v>
       </c>
-      <c r="K25" t="n">
+      <c r="N25" t="n">
         <v>30769</v>
       </c>
     </row>
@@ -1626,42 +1857,51 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>32191544</v>
+      </c>
+      <c r="E26" t="n">
+        <v>32191544</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>rs9469093</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>9.18302 (1.23027, 68.5443)</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
         <v>0.0306162</v>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H26" t="n">
+      <c r="K26" t="n">
         <v>0.8012563980959789</v>
       </c>
-      <c r="I26" t="n">
+      <c r="L26" t="n">
         <v>0</v>
       </c>
-      <c r="J26" t="n">
+      <c r="M26" t="n">
         <v>0.8012563980959789</v>
       </c>
-      <c r="K26" t="n">
+      <c r="N26" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1673,42 +1913,51 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>32186348</v>
+      </c>
+      <c r="E27" t="n">
+        <v>32405865</v>
+      </c>
+      <c r="F27" t="n">
+        <v>87</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>rs379464</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>NAT</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>0.0170609 (0.000322602, 0.902267)</t>
         </is>
       </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
         <v>0.0443506</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="H27" t="n">
+      <c r="K27" t="n">
         <v>-0.1422853250329177</v>
       </c>
-      <c r="I27" t="n">
+      <c r="L27" t="n">
         <v>0.006702176462369657</v>
       </c>
-      <c r="J27" t="n">
+      <c r="M27" t="n">
         <v>-0.1445393989897263</v>
       </c>
-      <c r="K27" t="n">
+      <c r="N27" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1720,42 +1969,51 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>34839925</v>
+      </c>
+      <c r="E28" t="n">
+        <v>35662319</v>
+      </c>
+      <c r="F28" t="n">
+        <v>13</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>rs9972241</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>0.970131 (0.946848, 0.993986)</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
         <v>0.01442</v>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>chr14</t>
         </is>
       </c>
-      <c r="H28" t="n">
+      <c r="K28" t="n">
         <v>0.02464890816420632</v>
       </c>
-      <c r="I28" t="n">
+      <c r="L28" t="n">
         <v>0.06949486463827942</v>
       </c>
-      <c r="J28" t="n">
+      <c r="M28" t="n">
         <v>0.00458961670881205</v>
       </c>
-      <c r="K28" t="n">
+      <c r="N28" t="n">
         <v>420084</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added allele in table
</commit_message>
<xml_diff>
--- a/tables_plots/table_fine_mapping.xlsx
+++ b/tables_plots/table_fine_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,35 +471,40 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>allele</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>OR (CI = 95%)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>p value</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>chr</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_mean</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_std</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_median</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_samples</t>
         </is>
@@ -537,27 +542,32 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>0.89809 (0.840833, 0.959245)</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>0.00138436</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>chr10</t>
         </is>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.01603793496567938</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.05794792982282904</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>-0.000309870533418</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>668</v>
       </c>
     </row>
@@ -593,27 +603,32 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>2.551 (1.40816, 4.62135)</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>0.00200839</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>chr9</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.2650826103238722</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.05520277919403747</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.2720060174950369</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>1065</v>
       </c>
     </row>
@@ -649,27 +664,32 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
           <t>0.844061 (0.80753, 0.882245)</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>5.917389999999999e-14</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>-0.02061823533022416</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.01964678905325687</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>-0.0254181746606881</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>36978</v>
       </c>
     </row>
@@ -705,27 +725,32 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
           <t>0.0506881 (0.00296067, 0.867803)</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>0.0396085</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>-0.04474911429178613</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.01495691423501778</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>-0.0484824113276277</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>81</v>
       </c>
     </row>
@@ -761,27 +786,32 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
           <t>1.53878 (1.03235, 2.29367)</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>0.0343209</v>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.06317405297773764</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.05684670391539608</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>0.0506722973675428</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>285</v>
       </c>
     </row>
@@ -817,27 +847,32 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>0.900401 (0.883096, 0.918046)</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>3.12314e-26</v>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>-0.02211802325627087</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.02136433981141503</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>-0.0257277744520354</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>27136</v>
       </c>
     </row>
@@ -873,27 +908,32 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
           <t>0.216515 (0.0645403, 0.726346)</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>0.013223</v>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>-0.1886719870376972</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.1076564051628712</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>-0.2313363699753964</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>22</v>
       </c>
     </row>
@@ -929,27 +969,32 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>0.0187251 (0.000562785, 0.623023)</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>0.0261095</v>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>-0.1325088443208639</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>0.00239733006487308</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>-0.1332971773429439</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>10</v>
       </c>
     </row>
@@ -985,27 +1030,32 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
           <t>0.905172 (0.838937, 0.976637)</t>
         </is>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>0.0101781</v>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.02657588963425587</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.1200299734152091</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>0.00677489475416395</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>902</v>
       </c>
     </row>
@@ -1041,27 +1091,32 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>129.955 (4.00638, 4215.35)</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>0.00611053</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>chr8</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0.008054595488127293</v>
       </c>
-      <c r="L11" t="n">
+      <c r="M11" t="n">
         <v>0.05792300338835416</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>3.527061131661646e-05</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>70</v>
       </c>
     </row>
@@ -1097,27 +1152,32 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
           <t>0.94514 (0.929624, 0.960916)</t>
         </is>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>2.38222e-11</v>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>-0.0116035395789694</v>
       </c>
-      <c r="L12" t="n">
+      <c r="M12" t="n">
         <v>0.02555237604918957</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>-0.0157108310070773</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>392123</v>
       </c>
     </row>
@@ -1153,27 +1213,32 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
           <t>1.42596 (1.2161, 1.67202)</t>
         </is>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>1.24933e-05</v>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0.02112058000943368</v>
       </c>
-      <c r="L13" t="n">
+      <c r="M13" t="n">
         <v>0.04195812000926728</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>0.0176744092042852</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>755</v>
       </c>
     </row>
@@ -1209,27 +1274,32 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
           <t>23.4192 (1.7359, 315.951)</t>
         </is>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>0.01753</v>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0.07240635403043384</v>
       </c>
-      <c r="L14" t="n">
+      <c r="M14" t="n">
         <v>0.09174849479652503</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>0.00260770984377</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1265,27 +1335,32 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
           <t>0.944111 (0.928517, 0.959967)</t>
         </is>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>1.3074e-11</v>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>-0.01164293497351661</v>
       </c>
-      <c r="L15" t="n">
+      <c r="M15" t="n">
         <v>0.02517480386191833</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>-0.01573311724271995</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>394378</v>
       </c>
     </row>
@@ -1321,27 +1396,32 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
           <t>19.9215 (1.56414, 253.728)</t>
         </is>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.0211924</v>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0.05555090371296323</v>
       </c>
-      <c r="L16" t="n">
+      <c r="M16" t="n">
         <v>0.07826594259621866</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>0.0005814157596602</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>33</v>
       </c>
     </row>
@@ -1377,27 +1457,32 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
           <t>0.883837 (0.863265, 0.904898)</t>
         </is>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>8.95268e-25</v>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>-0.01370129387070619</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M17" t="n">
         <v>0.02333677221547618</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>-0.0193954863883875</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>34786</v>
       </c>
     </row>
@@ -1433,27 +1518,32 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>1.62357 (1.11497, 2.36417)</t>
         </is>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>0.0114863</v>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>0.08061360773006593</v>
       </c>
-      <c r="L18" t="n">
+      <c r="M18" t="n">
         <v>0.06772259390299649</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>0.0735445606956977</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>271</v>
       </c>
     </row>
@@ -1489,27 +1579,32 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
           <t>1.05014 (1.03172, 1.06888)</t>
         </is>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>6.01662e-08</v>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>0.002848141718346069</v>
       </c>
-      <c r="L19" t="n">
+      <c r="M19" t="n">
         <v>0.02558179432450362</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>-0.0012338074059341</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>25287</v>
       </c>
     </row>
@@ -1545,27 +1640,32 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
           <t>0.0346081 (0.00196079, 0.610838)</t>
         </is>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>0.0216473</v>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>-0.1593371915749837</v>
       </c>
-      <c r="L20" t="n">
+      <c r="M20" t="n">
         <v>0.2086777729744027</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>-0.2464226786367025</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1601,27 +1701,32 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
           <t>0.0477015 (0.00332903, 0.683512)</t>
         </is>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>0.0250848</v>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>-0.1454155620917435</v>
       </c>
-      <c r="L21" t="n">
+      <c r="M21" t="n">
         <v>0.01945581826731453</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>-0.1539731871090594</v>
       </c>
-      <c r="N21" t="n">
+      <c r="O21" t="n">
         <v>9</v>
       </c>
     </row>
@@ -1657,27 +1762,32 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
           <t>0.987432 (0.976643, 0.99834)</t>
         </is>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>0.0240458</v>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
       </c>
-      <c r="K22" t="n">
+      <c r="L22" t="n">
         <v>0.003785101912323079</v>
       </c>
-      <c r="L22" t="n">
+      <c r="M22" t="n">
         <v>0.05990633516750271</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>-0.004835053114270901</v>
       </c>
-      <c r="N22" t="n">
+      <c r="O22" t="n">
         <v>1546</v>
       </c>
     </row>
@@ -1713,27 +1823,32 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
           <t>0.894641 (0.819604, 0.976549)</t>
         </is>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>0.012742</v>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>chr17</t>
         </is>
       </c>
-      <c r="K23" t="n">
+      <c r="L23" t="n">
         <v>-0.03679154899055308</v>
       </c>
-      <c r="L23" t="n">
+      <c r="M23" t="n">
         <v>0.07154148175801353</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>-0.02762697476021845</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>8776</v>
       </c>
     </row>
@@ -1769,27 +1884,32 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
           <t>1.71722 (1.1625, 2.53662)</t>
         </is>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>0.00659873</v>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K24" t="n">
+      <c r="L24" t="n">
         <v>0.08737157075405125</v>
       </c>
-      <c r="L24" t="n">
+      <c r="M24" t="n">
         <v>0.06810444311479932</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>0.07585703022469706</v>
       </c>
-      <c r="N24" t="n">
+      <c r="O24" t="n">
         <v>322</v>
       </c>
     </row>
@@ -1825,27 +1945,32 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
           <t>0.903429 (0.886177, 0.921016)</t>
         </is>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>5.49011e-25</v>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K25" t="n">
+      <c r="L25" t="n">
         <v>-0.02151903132644405</v>
       </c>
-      <c r="L25" t="n">
+      <c r="M25" t="n">
         <v>0.02189495770855255</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>-0.025199452815315</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>30769</v>
       </c>
     </row>
@@ -1881,27 +2006,32 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
           <t>9.18302 (1.23027, 68.5443)</t>
         </is>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>0.0306162</v>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K26" t="n">
+      <c r="L26" t="n">
         <v>0.8012563980959789</v>
       </c>
-      <c r="L26" t="n">
+      <c r="M26" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>0.8012563980959789</v>
       </c>
-      <c r="N26" t="n">
+      <c r="O26" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1937,27 +2067,32 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
           <t>0.0170609 (0.000322602, 0.902267)</t>
         </is>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>0.0443506</v>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="K27" t="n">
+      <c r="L27" t="n">
         <v>-0.1422853250329177</v>
       </c>
-      <c r="L27" t="n">
+      <c r="M27" t="n">
         <v>0.006702176462369657</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>-0.1445393989897263</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1993,27 +2128,32 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
           <t>0.970131 (0.946848, 0.993986)</t>
         </is>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>0.01442</v>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>chr14</t>
         </is>
       </c>
-      <c r="K28" t="n">
+      <c r="L28" t="n">
         <v>0.02464890816420632</v>
       </c>
-      <c r="L28" t="n">
+      <c r="M28" t="n">
         <v>0.06949486463827942</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>0.00458961670881205</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>420084</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rebuttal new analysis added
</commit_message>
<xml_diff>
--- a/tables_plots/table_fine_mapping.xlsx
+++ b/tables_plots/table_fine_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,20 +491,50 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Delta_P_mean</t>
+          <t>Delta_P_mean_ancestry</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Delta_P_std</t>
+          <t>Delta_P_median_ancestry</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Delta_P_median</t>
+          <t>Delta_P_std_ancestry</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_mean_add</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_median_add</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_std_add</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_mean_environment</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_median_environment</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Delta_P_std_environment</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Delta_P_samples</t>
         </is>
@@ -513,167 +543,203 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HC1007_TTE_acute_upper_respiratory_infections_of_multiple_and_unspecified_sites</t>
+          <t>HC221_Diabetes</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>AFR</t>
-        </is>
-      </c>
       <c r="D2" t="n">
-        <v>84405371</v>
+        <v>114596655</v>
       </c>
       <c r="E2" t="n">
-        <v>88296425</v>
+        <v>116330728</v>
       </c>
       <c r="F2" t="n">
-        <v>14</v>
+        <v>103</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>rs41307444</t>
+          <t>rs72826020</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>A</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.551 (1.40816, 4.62135)</t>
+          <t>0.89809 (0.840833, 0.959245)</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.00200839</v>
+        <v>0.00138436</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>chr9</t>
+          <t>chr10</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>-0.02456792082541624</v>
+        <v>0.001025297191886241</v>
       </c>
       <c r="M2" t="n">
-        <v>0.002319221512993106</v>
+        <v>0.0008178339195252</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.0251249993451782</v>
+        <v>0.0007614102076940834</v>
       </c>
       <c r="O2" t="n">
-        <v>1065</v>
+        <v>-0.01213260718979186</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-0.009637841997945699</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.009023424480940718</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.02433067442114763</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.007954337213032549</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.05789645533436961</v>
+      </c>
+      <c r="U2" t="n">
+        <v>668</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HC643_TTE_other_hypothyroidism</t>
+          <t>HC1007_TTE_acute_upper_respiratory_infections_of_multiple_and_unspecified_sites</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>AFR</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>30718180</v>
+        <v>84405371</v>
       </c>
       <c r="E3" t="n">
-        <v>31729925</v>
+        <v>88296425</v>
       </c>
       <c r="F3" t="n">
-        <v>1693</v>
+        <v>14</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>rs6931921</t>
+          <t>rs41307444</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0.844061 (0.80753, 0.882245)</t>
+          <t>2.551 (1.40816, 4.62135)</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>5.917389999999999e-14</v>
+        <v>0.00200839</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>chr6</t>
+          <t>chr9</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.00191503461430863</v>
+        <v>-0.02456792082541624</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0009872761530700823</v>
+        <v>-0.0251249993451782</v>
       </c>
       <c r="N3" t="n">
-        <v>0.00168583719601335</v>
+        <v>0.002319221512993106</v>
       </c>
       <c r="O3" t="n">
-        <v>36978</v>
+        <v>0.267929607130125</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.2763310701654379</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.04809921298175213</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-0.01023287529941413</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-0.010103347608871</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.03639093618056401</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1065</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HC1581_AD_asthma</t>
+          <t>HC643_TTE_other_hypothyroidism</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>EAS</t>
+          <t>EUR</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>32565979</v>
+        <v>30718180</v>
       </c>
       <c r="E4" t="n">
-        <v>32565979</v>
+        <v>31729925</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>1693</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>rs28383172</t>
+          <t>rs6931921</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1.53878 (1.03235, 2.29367)</t>
+          <t>0.844061 (0.80753, 0.882245)</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.0343209</v>
+        <v>5.917389999999999e-14</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -681,121 +747,157 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>-0.02247335741135638</v>
+        <v>0.00191503461430863</v>
       </c>
       <c r="M4" t="n">
-        <v>0.006936149992339912</v>
+        <v>0.00168583719601335</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0214556729836715</v>
+        <v>0.0009872761530700823</v>
       </c>
       <c r="O4" t="n">
-        <v>285</v>
+        <v>-0.01018927489228885</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0.008848585458942449</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.006435410835636327</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.008147770919041869</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-0.01268075658247255</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.01945659275271411</v>
+      </c>
+      <c r="U4" t="n">
+        <v>36978</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HC221_Diabetes</t>
+          <t>HC643_TTE_other_hypothyroidism</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>123760560</v>
+        <v>30809864</v>
       </c>
       <c r="E5" t="n">
-        <v>125664204</v>
+        <v>31141523</v>
       </c>
       <c r="F5" t="n">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>rs4128469</t>
+          <t>rs887468</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>T</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.905172 (0.838937, 0.976637)</t>
+          <t>0.0506881 (0.00296067, 0.867803)</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.0101781</v>
+        <v>0.0396085</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>chr8</t>
+          <t>chr6</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>-0.01335713232704032</v>
+        <v>0.005074192816415976</v>
       </c>
       <c r="M5" t="n">
-        <v>0.004735394436181141</v>
+        <v>0.0021603389337813</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0136998201504913</v>
+        <v>0.0117150251628845</v>
       </c>
       <c r="O5" t="n">
-        <v>902</v>
+        <v>-0.04474911429178613</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-0.0484824113276277</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.01495691423501778</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>81</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HC382_Asthma</t>
+          <t>HC1581_AD_asthma</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EUR</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>EAS</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>31480923</v>
+        <v>32565979</v>
       </c>
       <c r="E6" t="n">
-        <v>31480923</v>
+        <v>32565979</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>rs3131633</t>
+          <t>rs28383172</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>G</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>1.42596 (1.2161, 1.67202)</t>
+          <t>1.53878 (1.03235, 2.29367)</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>1.24933e-05</v>
+        <v>0.0343209</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -803,27 +905,45 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>-0.009210108058989377</v>
+        <v>-0.02247335741135638</v>
       </c>
       <c r="M6" t="n">
-        <v>0.001977288695265801</v>
+        <v>-0.0214556729836715</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.0091740980702154</v>
+        <v>0.006936149992339912</v>
       </c>
       <c r="O6" t="n">
-        <v>755</v>
+        <v>0.06224020021899396</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.0603985082211347</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.03148252672943738</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.001195761738441808</v>
+      </c>
+      <c r="S6" t="n">
+        <v>-0.0118847394874263</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.05459318130497166</v>
+      </c>
+      <c r="U6" t="n">
+        <v>285</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HC219_Hypothyroidism/myxoedema</t>
+          <t>HC1581_AD_asthma</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -832,17 +952,17 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>30628082</v>
+        <v>31435991</v>
       </c>
       <c r="E7" t="n">
-        <v>31729925</v>
+        <v>32565973</v>
       </c>
       <c r="F7" t="n">
-        <v>1790</v>
+        <v>1055</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Affx-28441669</t>
+          <t>rs4248166</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -852,11 +972,11 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.883837 (0.863265, 0.904898)</t>
+          <t>0.900401 (0.883096, 0.918046)</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>8.95268e-25</v>
+        <v>3.12314e-26</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -864,22 +984,40 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0.002271595814917757</v>
+        <v>-0.002631470119199209</v>
       </c>
       <c r="M7" t="n">
-        <v>0.001145773787476254</v>
+        <v>-0.00256697352605025</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0020093508341846</v>
+        <v>0.0004367473410662226</v>
       </c>
       <c r="O7" t="n">
-        <v>34786</v>
+        <v>-0.0193277324391254</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-0.0202343864569818</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.005613065503132442</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-0.002371965471695955</v>
+      </c>
+      <c r="S7" t="n">
+        <v>-0.0058601660724219</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.02114297508031006</v>
+      </c>
+      <c r="U7" t="n">
+        <v>27136</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HC382_Asthma</t>
+          <t>HC1581_AD_asthma</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -889,35 +1027,35 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EAS</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>31240771</v>
+        <v>31578772</v>
       </c>
       <c r="E8" t="n">
-        <v>31316699</v>
+        <v>31593476</v>
       </c>
       <c r="F8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>rs10484554</t>
+          <t>rs2844477</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>C</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1.62357 (1.11497, 2.36417)</t>
+          <t>0.216515 (0.0645403, 0.726346)</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0.0114863</v>
+        <v>0.013223</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -925,22 +1063,40 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>-0.02157916193474238</v>
+        <v>0.05789477875050254</v>
       </c>
       <c r="M8" t="n">
-        <v>0.006870461880455956</v>
+        <v>0.0435745547046591</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.021628504468022</v>
+        <v>0.0396479711931318</v>
       </c>
       <c r="O8" t="n">
-        <v>271</v>
+        <v>-0.1886719870376972</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.2313363699753964</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.1076564051628712</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FH1220_Diabetes_(FH)</t>
+          <t>HC1581_AD_asthma</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -950,21 +1106,21 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>NAT</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1795180</v>
+        <v>31435991</v>
       </c>
       <c r="E9" t="n">
-        <v>2282779</v>
+        <v>32413557</v>
       </c>
       <c r="F9" t="n">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>rs62067003</t>
+          <t>rs7758128</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -974,89 +1130,1547 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.894641 (0.819604, 0.976549)</t>
+          <t>0.0187251 (0.000562785, 0.623023)</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0.012742</v>
+        <v>0.0261095</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>chr17</t>
+          <t>chr6</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.01699530557858145</v>
+        <v>0.0005874117959682077</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0006974787044234969</v>
+        <v>3.906459835093074e-05</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0172114370517605</v>
+        <v>0.00166126929710058</v>
       </c>
       <c r="O9" t="n">
-        <v>8776</v>
+        <v>-0.1883230145693368</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-0.144298432557017</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.1522910853472826</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.0005576922344871503</v>
+      </c>
+      <c r="S9" t="n">
+        <v>5.325242115217608e-06</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.001637695259187727</v>
+      </c>
+      <c r="U9" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>HC221_Diabetes</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>123760560</v>
+      </c>
+      <c r="E10" t="n">
+        <v>125664204</v>
+      </c>
+      <c r="F10" t="n">
+        <v>35</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>rs4128469</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.905172 (0.838937, 0.976637)</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0101781</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>chr8</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>-0.01335713232704032</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-0.0136998201504913</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.004735394436181141</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-0.02311446625014551</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-0.0220962265213031</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.01402041822998241</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.04791597061942694</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.0276770729102144</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.1199500482133964</v>
+      </c>
+      <c r="U10" t="n">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HC221_Diabetes</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>124091971</v>
+      </c>
+      <c r="E11" t="n">
+        <v>124091971</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>rs4870843</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>129.955 (4.00638, 4215.35)</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0.00611053</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>chr8</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.0151052447194006</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-0.00033548632695585</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.05759869861342621</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.007680223397173196</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4.434092267676456e-06</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.05906980537629432</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.00467986306272371</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-1.197658982094667e-06</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.05758245469206603</v>
+      </c>
+      <c r="U11" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>31207822</v>
+      </c>
+      <c r="E12" t="n">
+        <v>31678691</v>
+      </c>
+      <c r="F12" t="n">
+        <v>618</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>rs2248372</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.94514 (0.929624, 0.960916)</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>2.38222e-11</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0.002861312434730673</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0027980238009143</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.0004729700779729219</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-0.00883691163812388</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-0.0083762923284014</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.004341951857642195</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-0.002538044447418575</v>
+      </c>
+      <c r="S12" t="n">
+        <v>-0.0066373228453341</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.02506644643808703</v>
+      </c>
+      <c r="U12" t="n">
+        <v>392123</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>31480923</v>
+      </c>
+      <c r="E13" t="n">
+        <v>31480923</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>rs3131633</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1.42596 (1.2161, 1.67202)</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>1.24933e-05</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>-0.009210108058989377</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-0.0091740980702154</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.001977288695265801</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.02527657901731842</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.0226747162549945</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.02776417762734456</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-0.004973398969273585</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-0.0059525114839263</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.03187848951240041</v>
+      </c>
+      <c r="U13" t="n">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>31330546</v>
+      </c>
+      <c r="E14" t="n">
+        <v>31371430</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>rs2596548</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>23.4192 (1.7359, 315.951)</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>0.01753</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>-0.1688583761362347</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-0.0416836813000412</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.1635284329974204</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.06750468655856032</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.0898717346065525</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.01567558425595559</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-0.0013824174438016</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.04957129523788515</v>
+      </c>
+      <c r="U14" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HC1581_AD_asthma</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>31207822</v>
+      </c>
+      <c r="E15" t="n">
+        <v>31570670</v>
+      </c>
+      <c r="F15" t="n">
+        <v>531</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>rs2248372</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.944111 (0.928517, 0.959967)</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>1.3074e-11</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>0.002472151022526098</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0024161015025238</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0004114068002486931</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-0.00886727348218415</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-0.008402070461490749</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.00436387106165081</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-0.002544258009902234</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-0.0066254738000417</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.0246874656033272</v>
+      </c>
+      <c r="U15" t="n">
+        <v>394378</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>HC1581_AD_asthma</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>31218268</v>
+      </c>
+      <c r="E16" t="n">
+        <v>31570670</v>
+      </c>
+      <c r="F16" t="n">
+        <v>25</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>rs2596548</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>19.9215 (1.56414, 253.728)</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0211924</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>-0.1464512364723784</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-0.0328449409421444</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1540314312890013</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.0511267729495286</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.07541487360912304</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.01391283148463814</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-0.0011905251041553</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.04373694046501374</v>
+      </c>
+      <c r="U16" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HC219_Hypothyroidism/myxoedema</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>30628082</v>
+      </c>
+      <c r="E17" t="n">
+        <v>31729925</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1790</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Affx-28441669</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0.883837 (0.863265, 0.904898)</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>8.95268e-25</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>0.002271595814917757</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.0020093508341846</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.001145773787476254</v>
+      </c>
+      <c r="O17" t="n">
+        <v>-0.003120049037733445</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-0.00222143132676685</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.003851332501033844</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-0.009922103014899115</v>
+      </c>
+      <c r="S17" t="n">
+        <v>-0.01544337483726835</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.02326783347725167</v>
+      </c>
+      <c r="U17" t="n">
+        <v>34786</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>EAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>31240771</v>
+      </c>
+      <c r="E18" t="n">
+        <v>31316699</v>
+      </c>
+      <c r="F18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>rs10484554</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1.62357 (1.11497, 2.36417)</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0114863</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>-0.02157916193474238</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-0.021628504468022</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.006870461880455956</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.07869409359598313</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.07193831286173021</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.04110261947108181</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.0003592821170134407</v>
+      </c>
+      <c r="S18" t="n">
+        <v>-0.0041873367299903</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.06197336684942346</v>
+      </c>
+      <c r="U18" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>31229579</v>
+      </c>
+      <c r="E19" t="n">
+        <v>32565973</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1435</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>rs9266490</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1.05014 (1.03172, 1.06888)</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>6.01662e-08</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>-0.002859729313861368</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.0027996654818359</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.0004578513734539174</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.005396698779906562</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.0052954756732368</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.003423267157779086</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-0.002652289118431702</v>
+      </c>
+      <c r="S19" t="n">
+        <v>-0.0066182408403163</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.02524578597983267</v>
+      </c>
+      <c r="U19" t="n">
+        <v>25287</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>31266767</v>
+      </c>
+      <c r="E20" t="n">
+        <v>31628733</v>
+      </c>
+      <c r="F20" t="n">
+        <v>9</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>rs4394275</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.0346081 (0.00196079, 0.610838)</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>0.0216473</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>0.02797899830431218</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.00052012145165695</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.05643416257293231</v>
+      </c>
+      <c r="O20" t="n">
+        <v>-0.3212079193612197</v>
+      </c>
+      <c r="P20" t="n">
+        <v>-0.2176004067169831</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.282426976468739</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.07488352331320444</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.00037641061108965</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.1976111326129406</v>
+      </c>
+      <c r="U20" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>HC382_Asthma</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>31236800</v>
+      </c>
+      <c r="E21" t="n">
+        <v>32413557</v>
+      </c>
+      <c r="F21" t="n">
+        <v>86</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>rs13198903</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.0477015 (0.00332903, 0.683512)</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0250848</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>0.006031374732711255</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.0002601817741408</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.01345864786599402</v>
+      </c>
+      <c r="O21" t="n">
+        <v>-0.1675752396782036</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-0.1308615816110415</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.1392307548538185</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.005664970108409667</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-0.0001097769295173</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.01999308274682543</v>
+      </c>
+      <c r="U21" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FH1220_Diabetes_(FH)</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1605567</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2307902</v>
+      </c>
+      <c r="F22" t="n">
+        <v>23</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>rs903160</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.987432 (0.976643, 0.99834)</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0240458</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>chr17</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>0.002924609223392237</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.00290741248484925</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.0004719078103369899</v>
+      </c>
+      <c r="O22" t="n">
+        <v>-0.002799468129119684</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-0.0024704490830662</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.001626215616102643</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.006587627600063759</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.0021963340590169</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0.05991421715700439</v>
+      </c>
+      <c r="U22" t="n">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FH1220_Diabetes_(FH)</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1795180</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2282779</v>
+      </c>
+      <c r="F23" t="n">
+        <v>17</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>rs62067003</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.894641 (0.819604, 0.976549)</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0.012742</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>chr17</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>0.01699530557858145</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.0172114370517605</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.0006974787044234969</v>
+      </c>
+      <c r="O23" t="n">
+        <v>-0.04673589394656425</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-0.0540372385100332</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.01332533861007875</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.01105604480006623</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.01980564038282225</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0.06976192439252711</v>
+      </c>
+      <c r="U23" t="n">
+        <v>8776</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>HC1036_TTE_asthma</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>SAS</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>EAS</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D24" t="n">
         <v>32565979</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E24" t="n">
         <v>32565979</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F24" t="n">
         <v>1</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>rs28383172</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>1.71722 (1.1625, 2.53662)</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="J24" t="n">
         <v>0.00659873</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>chr6</t>
         </is>
       </c>
-      <c r="L10" t="n">
+      <c r="L24" t="n">
         <v>-0.02360223409644694</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M24" t="n">
+        <v>-0.02317015070367895</v>
+      </c>
+      <c r="N24" t="n">
         <v>0.007288919122936892</v>
       </c>
-      <c r="N10" t="n">
-        <v>-0.02317015070367895</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="O24" t="n">
+        <v>0.08591880081793046</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.07834404259779836</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.04398091162167017</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-0.001154103434816279</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.0051048210853399</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0.06251309442139863</v>
+      </c>
+      <c r="U24" t="n">
         <v>322</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>HC1036_TTE_asthma</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>32177880</v>
+      </c>
+      <c r="E25" t="n">
+        <v>32565973</v>
+      </c>
+      <c r="F25" t="n">
+        <v>528</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>rs4248166</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.903429 (0.886177, 0.921016)</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>5.49011e-25</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>-0.002272793811841412</v>
+      </c>
+      <c r="M25" t="n">
+        <v>-0.0022180996521902</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.0003748895107019773</v>
+      </c>
+      <c r="O25" t="n">
+        <v>-0.01908987765326004</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-0.0200094906947855</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.005564230957669202</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-0.002070520303381757</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-0.005726701773005</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0.02169965329194964</v>
+      </c>
+      <c r="U25" t="n">
+        <v>30769</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>HC1036_TTE_asthma</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>32191544</v>
+      </c>
+      <c r="E26" t="n">
+        <v>32191544</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>rs9469093</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>9.18302 (1.23027, 68.5443)</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>0.0306162</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>0.0738192535302</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.0738192535302</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.8012563980959789</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.8012563980959789</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>HC1036_TTE_asthma</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NAT</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>32186348</v>
+      </c>
+      <c r="E27" t="n">
+        <v>32405865</v>
+      </c>
+      <c r="F27" t="n">
+        <v>87</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>rs379464</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>0.0170609 (0.000322602, 0.902267)</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>0.0443506</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>chr6</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>0.001617197946802504</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1.943424632908296e-05</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.004826012123903434</v>
+      </c>
+      <c r="O27" t="n">
+        <v>-0.123290913228133</v>
+      </c>
+      <c r="P27" t="n">
+        <v>-0.0827027028071628</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.1500489694906739</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.001793849447892432</v>
+      </c>
+      <c r="S27" t="n">
+        <v>-2.533946551828086e-05</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.006926966799696762</v>
+      </c>
+      <c r="U27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>HC221_Diabetes</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>34839925</v>
+      </c>
+      <c r="E28" t="n">
+        <v>35662319</v>
+      </c>
+      <c r="F28" t="n">
+        <v>13</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>rs9972241</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0.970131 (0.946848, 0.993986)</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>0.01442</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>chr14</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>-0.001203016300500977</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-0.00094909807274925</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.0009163262962785816</v>
+      </c>
+      <c r="O28" t="n">
+        <v>-0.003122098656557636</v>
+      </c>
+      <c r="P28" t="n">
+        <v>-0.00236027932338125</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.002656660801339537</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.02680280106228063</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.00674113939441975</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.06948600268087646</v>
+      </c>
+      <c r="U28" t="n">
+        <v>420084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>